<commit_message>
images updates, kontent score updates
</commit_message>
<xml_diff>
--- a/CMS Recommendations.xlsx
+++ b/CMS Recommendations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\zMyFiles\Personal Files\TestProjects\CMS\CMS-Recommendation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04030EB2-9A8A-4C26-AF2C-83D7A2DF6994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB8B6E1-DB79-45A5-8904-4A9FE5F6AE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" xr2:uid="{3D53F9EC-C185-4C3E-ACB6-AF20BA6D9148}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3D53F9EC-C185-4C3E-ACB6-AF20BA6D9148}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -317,7 +317,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,23 +660,23 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="74.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="74.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
@@ -695,8 +695,8 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -710,7 +710,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -730,7 +730,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -750,7 +750,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -790,8 +790,8 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -805,7 +805,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -816,7 +816,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="3">
         <v>10</v>
@@ -825,7 +825,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -836,7 +836,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" s="3">
         <v>9</v>
@@ -845,7 +845,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -865,7 +865,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -885,8 +885,8 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -900,7 +900,7 @@
       <c r="G15" s="6"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -911,7 +911,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E16" s="3">
         <v>10</v>
@@ -920,7 +920,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -940,7 +940,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -960,7 +960,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -980,8 +980,8 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>22</v>
       </c>
@@ -995,7 +995,7 @@
       <c r="G21" s="6"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="3">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E22" s="3">
         <v>7</v>
@@ -1015,7 +1015,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -1035,7 +1035,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -1055,7 +1055,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -1075,8 +1075,8 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>28</v>
       </c>
@@ -1090,7 +1090,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="3">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E28" s="3">
         <v>7</v>
@@ -1110,7 +1110,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
@@ -1130,7 +1130,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>32</v>
       </c>
@@ -1150,7 +1150,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
@@ -1172,8 +1172,8 @@
       </c>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>35</v>
       </c>
@@ -1187,7 +1187,7 @@
       <c r="G33" s="6"/>
       <c r="H33" s="7"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>36</v>
       </c>
@@ -1227,7 +1227,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>37</v>
       </c>
@@ -1247,7 +1247,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>38</v>
       </c>
@@ -1267,8 +1267,8 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>48</v>
       </c>
@@ -1282,7 +1282,7 @@
       <c r="G39" s="6"/>
       <c r="H39" s="7"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>41</v>
       </c>
@@ -1302,7 +1302,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>42</v>
       </c>
@@ -1322,12 +1322,12 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B42" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C42" s="3">
         <v>9</v>
@@ -1342,7 +1342,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
@@ -1362,8 +1362,8 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>49</v>
       </c>
@@ -1377,7 +1377,7 @@
       <c r="G45" s="6"/>
       <c r="H45" s="7"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>24</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>25</v>
       </c>
@@ -1417,7 +1417,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>

</xml_diff>